<commit_message>
Scrapping completed for Nykaa,Amazon,Myntra and Tira
</commit_message>
<xml_diff>
--- a/Scraped_Product_Prices.xlsx
+++ b/Scraped_Product_Prices.xlsx
@@ -493,17 +493,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/10861588/</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.tirabeauty.com/products/?q=961292</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://blinkit.com/prn/m/prid/504593/</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -518,12 +518,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>795</t>
+          <t>https://www.nykaa.com/mak/p/7883823</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>795</t>
+          <t>https://www.amazon.in/dp/B08YHT369B</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.tirabeauty.com/products/?q=1151976</t>
+          <t>https://www.tirabeauty.com/product/makeup-revolution-fix-glow-fixing-spray-100-ml-7605368</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -553,12 +553,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1540</t>
+          <t>https://www.nykaa.com/makeup-revolution-forever-flawless/p/4241822?redirectpath=slug&amp;skuId=646072</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1435</t>
+          <t>https://www.amazon.in/dp/B07ZWC2NJ9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.tirabeauty.com/products/?q=1160851</t>
+          <t>https://www.tirabeauty.com/product/makeup-revolution-the-icon-palette-enchanted-icon-8-4-g-7615083</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.tirabeauty.com/products/?q=1160797</t>
+          <t>https://www.tirabeauty.com/product/makeup-revolution-pout-bomb-plumping-gloss-rosewood-rose-pink-4-6-ml-7615088</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -623,12 +623,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>946</t>
+          <t>https://www.nykaa.com/mak/p/2725253</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B08T6Z75L9</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.tirabeauty.com/products/?q=1124431</t>
+          <t>https://www.tirabeauty.com/product/makeup-revolution-streamline-waterline-eyeliner-pencil-brown-1-3g-7572797</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -660,12 +660,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81859/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1058</t>
+          <t>https://www.amazon.in/dp/B01M4IGE0Y</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1670</t>
+          <t>https://www.nykaa.com/l/p/1374361</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -734,12 +734,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40870</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>711</t>
+          <t>https://www.amazon.in/dp/B007MJKHVO</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -771,12 +771,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40872</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B007MJKHZ0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -808,12 +808,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-concealer-color-corrector/p/81924?redirectpath=slug&amp;skuId=81882</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>572</t>
+          <t>https://www.amazon.in/dp/B01LXJHM36</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -843,12 +843,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1575</t>
+          <t>https://www.nykaa.com/makeup-revolution-forever-flawless-palette/p/18283926?productId=18283926&amp;pps=1&amp;skuId=18283921</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1575</t>
+          <t>https://www.amazon.in/dp/B0DHL2ZD6R</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -878,12 +878,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1076</t>
+          <t>https://www.nykaa.com/mak/p/18283922</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1076</t>
+          <t>https://www.amazon.in/dp/B0D1R7KM3H</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -915,12 +915,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>https://www.nykaa.com/focallure-color-lasting-lip-tint/p/18238936?productId=18238936&amp;pps=1&amp;skuId=18238927</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>733</t>
+          <t>https://www.amazon.in/dp/B08QHX26MP</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -950,12 +950,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>629</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=354049</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>629</t>
+          <t>https://www.amazon.in/dp/B07FZK5B3P</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -987,12 +987,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/mak/p/626231</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1062</t>
+          <t>https://www.amazon.in/dp/B07YGQYNSJ</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1022,12 +1022,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>808</t>
+          <t>https://www.nykaa.com/mak/p/913428</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>https://www.amazon.in/dp/B081X3KTGW</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1059,12 +1059,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>874</t>
+          <t>https://www.nykaa.com/mak/p/40892</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>855</t>
+          <t>https://www.amazon.in/dp/B00PGQYEUK</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1094,12 +1094,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>723</t>
+          <t>https://www.nykaa.com/makeup-revolution-cheek-kit/p/465893?redirectpath=slug&amp;skuId=465889</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>595</t>
+          <t>https://www.amazon.in/dp/B07QNWFHVR</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1129,12 +1129,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>459</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-roll-baby-lip-oil/p/8465696?redirectpath=slug&amp;skuId=8465680</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>https://www.amazon.in/dp/B0BJW3C7XN</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1164,12 +1164,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237978</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>https://www.amazon.in/dp/B0DSWM222H</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1199,12 +1199,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/l/p/12098248?redirectpath=slug&amp;skuId=12098223</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.amazon.in/dp/B0C9ZFSC9D</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1234,12 +1234,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>https://www.nykaa.com/makeup-revolution-jelly-blush-stick/p/19145036?redirectpath=slug&amp;skuId=18236799</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>https://www.amazon.in/dp/B0DCZJBCL3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1271,12 +1271,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/mak/p/626232</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>https://www.amazon.in/dp/B07ZDWKJH1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>https://www.nykaa.com/makeup-revolution-jelly-blush-stick/p/19145036?redirectpath=slug&amp;skuId=18236798</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>https://www.amazon.in/dp/B0DCZNC6HZ</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1341,12 +1341,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.nykaa.com/lamel-all-in-one-lip-tinted-plumping-oil/p/12268696?productId=12268696&amp;pps=2&amp;skuId=12268622</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>https://www.amazon.in/dp/B0B56W3LJW</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1378,12 +1378,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40867</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B007MJKHPA</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1415,12 +1415,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81858</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>https://www.amazon.in/dp/B01M8HNHAK</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1450,12 +1450,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>https://www.nykaa.com/mak/p/12268658</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>https://www.amazon.in/dp/B0B56YDHFH</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1487,12 +1487,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81861</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>https://www.amazon.in/dp/B01MF71U77</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1522,12 +1522,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237975</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>https://www.amazon.in/dp/B0DSWMGN6Z</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1063</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18498580</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1655</t>
+          <t>https://www.nykaa.com/l/p/4308959?redirectpath=slug&amp;skuId=775532</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1627,12 +1627,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>459</t>
+          <t>https://www.nykaa.com/mak/p/3887837</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B07VRLPNY1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1662,12 +1662,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>https://www.nykaa.com/lamel-stain-hydrating-lip-tint/p/19011219?redirectpath=slug&amp;skuId=19011218</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>625</t>
+          <t>https://www.amazon.in/dp/B0DTKMYZTS</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.nykaa.com/lamel-all-in-one-lip-tinted-plumping-oil/p/12268696?productId=12268696&amp;pps=2&amp;skuId=14406214</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>401</t>
+          <t>https://www.amazon.in/dp/B0CR6XMZ26</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1734,12 +1734,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>823</t>
+          <t>https://www.nykaa.com/focallure-airy-velvet-lipcream/p/17516493?productId=17516493&amp;pps=1&amp;skuId=17516458</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>https://www.amazon.in/dp/B08MKZ9112</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1769,12 +1769,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1076</t>
+          <t>https://www.nykaa.com/makeup-revolution-eyeshadow-palette/p/17523809?redirectpath=slug&amp;skuId=17523802</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>837</t>
+          <t>https://www.amazon.in/dp/B0D1R67516</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>https://www.nykaa.com/mak/p/302275</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/mak/p/7883822</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>920</t>
+          <t>https://www.nykaa.com/mak/p/156472</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DXL57BJT</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1946,12 +1946,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>https://www.nykaa.com/focallure-color-lasting-lip-tint/p/18238936?productId=18238936&amp;pps=1&amp;skuId=18238925</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>https://www.amazon.in/dp/B08QHXR6J4</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1981,12 +1981,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/l/p/12098248?redirectpath=slug&amp;skuId=12098226</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>276</t>
+          <t>https://www.amazon.in/dp/B0C9ZD2WX4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/makeup-revolution-superdewy-liquid-blush/p/3861510?productId=3861510&amp;pps=1&amp;skuId=3753869</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>https://www.amazon.in/dp/B08NDCBZ42</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2088,12 +2088,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>367</t>
+          <t>https://www.nykaa.com/revolution-relove-baby-tint-coral-lip-cheek-tint/p/4349383?redirectpath=slug&amp;skuId=4349379</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>294</t>
+          <t>https://www.amazon.in/dp/B09NGMQ2HT</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237976</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2160,12 +2160,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/mak/p/288547</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.amazon.in/dp/B07B6GFC8L</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>https://www.nykaa.com/mak/p/8518902</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2232,12 +2232,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40877</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>572</t>
+          <t>https://www.amazon.in/dp/B009WI05BU</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2269,12 +2269,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40866</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>695</t>
+          <t>https://www.amazon.in/dp/B007MJKHN2</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2306,12 +2306,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40876</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B009WI04PM</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DXL3R8YY</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2376,12 +2376,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-baby-gloss/p/8465698?redirectpath=slug&amp;skuId=8465689</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>https://www.amazon.in/dp/B095HZTZ2V</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2413,12 +2413,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>https://www.nykaa.com/focallure-color-lasting-lip-tint/p/18238936?productId=18238936&amp;pps=1&amp;skuId=18238926</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>811</t>
+          <t>https://www.amazon.in/dp/B08QHYB7J9</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2448,12 +2448,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>945</t>
+          <t>https://www.nykaa.com/makeup-revolution-ultra-blush-and-contour-palette/p/24735?redirectpath=slug&amp;skuId=24738</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>945</t>
+          <t>https://www.amazon.in/dp/B00TFQASF2</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1665</t>
+          <t>https://www.nykaa.com/l/p/5237373</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2522,12 +2522,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-face-pressed-powder/p/41449?redirectpath=slug&amp;skuId=61584</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>https://www.amazon.in/dp/B01E1SL7BM</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2559,7 +2559,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>823</t>
+          <t>https://www.nykaa.com/focallure-airy-velvet-lipcream/p/17516493?productId=17516493&amp;pps=1&amp;skuId=17516453</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/revolution-pro-4k-highlighter-palette/p/343102?productId=343102&amp;pps=1&amp;skuId=343100</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1439</t>
+          <t>https://www.nykaa.com/l/p/4308959?redirectpath=slug&amp;skuId=664449</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2664,12 +2664,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237979</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.amazon.in/dp/B0DZNYRSVV</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B08R3M55Q7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2738,12 +2738,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1058</t>
+          <t>https://www.nykaa.com/mak/p/514178</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>893</t>
+          <t>https://www.amazon.in/dp/B01DQ3GYAC</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2773,12 +2773,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/lamel-lamination-brow-lash-gel-401-transparent/p/12268685?productId=12268685&amp;pps=1</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>https://www.amazon.in/dp/B0B1Z6V23T</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81865</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2847,12 +2847,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81862</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>https://www.amazon.in/dp/B01MA35XN6</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2884,12 +2884,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40886</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>https://www.amazon.in/dp/B00VKKJ2I0</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2921,12 +2921,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>736</t>
+          <t>https://www.nykaa.com/mak/p/326897</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>736</t>
+          <t>https://www.amazon.in/dp/B07D51LP6X</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2958,12 +2958,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-bb-cream/p/41499?redirectpath=slug&amp;skuId=41500</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>https://www.amazon.in/dp/B00NQI6GGU</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2995,12 +2995,12 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/mak/p/41447</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.amazon.in/dp/B01E1SL9R4</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1240</t>
+          <t>https://www.nykaa.com/mak/p/3887825</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3067,12 +3067,12 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-color-foundation/p/378199?redirectpath=slug&amp;skuId=378196</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1125</t>
+          <t>https://www.amazon.in/dp/B07HPF4TNB</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3104,12 +3104,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>595</t>
+          <t>https://www.nykaa.com/mak/p/8318254</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0BDRHJLTC</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3139,12 +3139,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-baby-gloss/p/8465698?redirectpath=slug&amp;skuId=8465690</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>https://www.amazon.in/dp/B095J1NC7W</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/makeup-revolution-pro-4k-blush-palette-peach/p/445861?productId=445861&amp;pps=1</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3209,12 +3209,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237980</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>https://www.amazon.in/dp/B0DSWMYY91</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>553</t>
+          <t>https://www.nykaa.com/mak/p/3887833</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3279,12 +3279,12 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>https://www.nykaa.com/mak/p/2784821</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>https://www.amazon.in/dp/B095HZ1K8V</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3314,12 +3314,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>855</t>
+          <t>https://www.nykaa.com/mak/p/8518895</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B07NGR137Q</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1016</t>
+          <t>https://www.nykaa.com/makeup-revolution-eyeshadow-palette/p/17523809?redirectpath=slug&amp;skuId=17523801</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/mak/p/2725254</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B07VP3XY58</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -3456,12 +3456,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>https://www.nykaa.com/lamel-stain-hydrating-lip-tint/p/19011219?redirectpath=slug&amp;skuId=19011216</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DTKND7KV</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.amazon.in/dp/B08QYP1QFL</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3528,12 +3528,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>https://www.nykaa.com/revolution-relove-baby-tint-coral-lip-cheek-tint/p/4349383?redirectpath=slug&amp;skuId=4349378</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>https://www.amazon.in/dp/B09NGVVWPV</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3563,12 +3563,12 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>https://www.nykaa.com/makeup-revolution-blusher-reloaded/p/540752?redirectpath=slug&amp;skuId=540750</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B07WDCWWWT</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>723</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-bb-cream/p/41499?productId=41499&amp;pps=1&amp;skuId=41501</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3637,12 +3637,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40864</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>https://www.amazon.in/dp/B00VKIJPNE</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3674,12 +3674,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-face-pressed-powder/p/41449?redirectpath=slug&amp;skuId=41448</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B01N0EMO4Q</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3711,12 +3711,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40885</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B00VKKJ01Y</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3748,12 +3748,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>https://www.nykaa.com/focallure-fa-l12-glisten-opal-hydrating-lip-balm/p/17516498?productId=17516498&amp;pps=1&amp;skuId=17516480</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>https://www.amazon.in/dp/B08NT6M6PS</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3785,12 +3785,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=378183</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>https://www.amazon.in/dp/B07HR5BV5L</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3822,12 +3822,12 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>https://www.nykaa.com/focallure-color-lasting-lip-tint/p/18238936?productId=18238936&amp;pps=1&amp;skuId=18238928</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>https://www.amazon.in/dp/B08QHW3JKR</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3857,12 +3857,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>723</t>
+          <t>https://www.nykaa.com/makeup-revolution-cheek-kit/p/465893?redirectpath=slug&amp;skuId=465892</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>https://www.amazon.in/dp/B07QPY1RVC</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3894,12 +3894,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.nykaa.com/pinkflash-watery-transferproof-lip-tint/p/19132338?productId=19132338&amp;pps=1&amp;skuId=19132331</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.amazon.in/dp/B08QYMYGNL</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-conceal-hd/p/40862?redirectpath=slug&amp;skuId=40863</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3966,7 +3966,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.nykaa.com/lamel-all-in-one-lip-tinted-plumping-oil/p/12268696?productId=12268696&amp;pps=1&amp;skuId=12268623</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4001,12 +4001,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>https://www.nykaa.com/makeup-revolution-blusher-reloaded/p/540752?redirectpath=slug&amp;skuId=540751</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>https://www.amazon.in/dp/B07VQQRR7W</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -4036,12 +4036,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>https://www.nykaa.com/lamel-stain-hydrating-lip-tint/p/19011219?redirectpath=slug&amp;skuId=19011215</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>https://www.amazon.in/dp/B0DTKLQLNZ</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4071,7 +4071,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>808</t>
+          <t>https://www.nykaa.com/mak/p/28733</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4106,12 +4106,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.nykaa.com/makeup-revolution-fast-base-contour-stick/p/6832681?productId=6832681&amp;pps=1&amp;skuId=6832630</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>556</t>
+          <t>https://www.amazon.in/dp/B0B5PR2TN5</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4141,14 +4141,10 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>629</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=1319459</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
           <t>https://www.myntra.com/23630022/</t>
@@ -4176,12 +4172,12 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>638</t>
+          <t>https://www.nykaa.com/makeup-revolution-pout-tint/p/15662756?redirectpath=slug&amp;skuId=15662739</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>https://www.amazon.in/dp/B0CT474XG1</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -4211,12 +4207,12 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.nykaa.com/lamel-all-in-one-lip-tinted-plumping-oil/p/12268696?productId=12268696&amp;pps=2&amp;skuId=14406215</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.amazon.in/dp/B0CR6VXP8X</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -4246,7 +4242,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=497424</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4281,7 +4277,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237977</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4318,7 +4314,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40881</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4355,7 +4351,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>713</t>
+          <t>https://www.nykaa.com/l-a-girl-luminous-glow-illuminating-cream/p/306042?productId=306042&amp;pps=1&amp;skuId=306040</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4390,7 +4386,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>https://www.nykaa.com/makeup-revolution-forever-flawless/p/4241822?redirectpath=slug&amp;skuId=2725255</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -4425,7 +4421,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=497425</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -4462,12 +4458,12 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40873</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B007MJKI22</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -4497,7 +4493,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/mak/p/3753870</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -4534,12 +4530,12 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>https://www.nykaa.com/pinkflash-watery-transferproof-lip-tint/p/19132338?productId=19132338&amp;pps=1&amp;skuId=19132334</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>611</t>
+          <t>https://www.amazon.in/dp/B08R3MRSHL</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -4569,12 +4565,12 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>459</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-roll-baby-lip-oil/p/8465696?redirectpath=slug&amp;skuId=8465678</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>459</t>
+          <t>https://www.amazon.in/dp/B0BJW24KG7</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4604,12 +4600,12 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>https://www.nykaa.com/mak/p/2784813</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>https://www.amazon.in/dp/B095J1WCR6</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -4639,7 +4635,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>https://www.nykaa.com/mak/p/465898</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4674,12 +4670,12 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>https://www.nykaa.com/lamel-let-s-glaze-hydrating-lip-oil/p/17269856?redirectpath=slug&amp;skuId=17269855</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>440</t>
+          <t>https://www.amazon.in/dp/B0D7WGVKRZ</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -4709,12 +4705,12 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236971</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DZN887S3</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -4744,7 +4740,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>855</t>
+          <t>https://www.nykaa.com/makeup-revolution-loose-baking-powder/p/8518928?redirectpath=slug&amp;skuId=8518865</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4781,7 +4777,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1670</t>
+          <t>https://www.nykaa.com/l/p/1374360</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4818,7 +4814,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>825</t>
+          <t>https://www.nykaa.com/mak/p/784956</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4853,7 +4849,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=269786</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4888,12 +4884,12 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>1655</t>
+          <t>https://www.nykaa.com/l/p/4308959?redirectpath=slug&amp;skuId=3753872</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>1295</t>
+          <t>https://www.amazon.in/dp/B09BRZHJS1</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -4923,7 +4919,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=18283941</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4960,12 +4956,12 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>https://www.nykaa.com/mak/p/41498</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.amazon.in/dp/B00WNCS852</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -4997,12 +4993,12 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40878</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>https://www.amazon.in/dp/B009WI06DC</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -5034,7 +5030,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-face-pressed-powder/p/41449?redirectpath=slug&amp;skuId=41452</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -5069,12 +5065,12 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>708</t>
+          <t>https://www.nykaa.com/makeup-revolution-beam-bright-highlighter/p/15662754?redirectpath=slug&amp;skuId=15662728</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/need to list</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -5106,7 +5102,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-face-pressed-powder/p/41449?redirectpath=slug&amp;skuId=61583</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -5141,12 +5137,12 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>https://www.nykaa.com/mak/p/2784825</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>https://www.amazon.in/dp/B095J1YZ59</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -5178,12 +5174,12 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.nykaa.com/pinkflash-watery-transferproof-lip-tint/p/19132338?productId=19132338&amp;pps=1&amp;skuId=19132335</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>https://www.amazon.in/dp/B08R3MTCCX</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5213,12 +5209,12 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>https://www.nykaa.com/mak/p/2784843</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>339</t>
+          <t>https://www.amazon.in/dp/B09J2M3RYM</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -5250,7 +5246,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40880</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -5285,12 +5281,12 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/l/p/12098248?redirectpath=slug&amp;skuId=12098224</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.amazon.in/dp/B0C9ZH7C38</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5322,12 +5318,12 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81864</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>https://www.amazon.in/dp/B01M7P05PX</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -5357,7 +5353,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>639</t>
+          <t>https://www.nykaa.com/mak/p/11958425</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -5392,7 +5388,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>713</t>
+          <t>https://www.nykaa.com/mak/p/24736</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -5429,12 +5425,12 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81860</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>https://www.amazon.in/dp/B01MA35R47</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -5464,7 +5460,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>https://www.nykaa.com/lamel-let-s-glaze-hydrating-lip-oil/p/17269856?productId=17269856&amp;pps=1&amp;skuId=17269854</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -5499,7 +5495,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237981</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -5534,12 +5530,12 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>322</t>
+          <t>https://www.nykaa.com/relove-colour-play-blushed-duo/p/3442503?productId=3442503&amp;pps=1&amp;skuId=2784793</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>https://www.amazon.in/dp/B09J2LMG2X</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -5569,7 +5565,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>https://www.nykaa.com/xx-revolution-xx-shadow-palette-xxplosion/p/1427340?productId=1427340&amp;pps=9</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -5641,12 +5637,13 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236970</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/
+  B0DZNX4F4S</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -5676,12 +5673,12 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236974</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.amazon.in/dp/B0DZNDYTYV</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -5711,12 +5708,12 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>405</t>
+          <t>https://www.nykaa.com/mak/p/12268635</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>382</t>
+          <t>https://www.amazon.in/dp/B09SXFXNVS</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -5748,7 +5745,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>1233</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81868</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -5783,12 +5780,12 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-baby-gloss/p/8465698?redirectpath=slug&amp;skuId=8465691</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>https://www.amazon.in/dp/B095J2Q4TN</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -5818,12 +5815,12 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/l/p/12098248?redirectpath=slug&amp;skuId=12098225</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>https://www.amazon.in/dp/B0C9ZFL8RH</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -5853,7 +5850,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/mak/p/2637681</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -5888,12 +5885,12 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>https://www.nykaa.com/l/p/12098248?redirectpath=slug&amp;skuId=12098222</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>343</t>
+          <t>https://www.amazon.in/dp/B0C9ZFT9W9</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -5923,7 +5920,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>https://www.nykaa.com/makeup-revolution-fast-base-stick-foundation/p/302292?redirectpath=slug&amp;skuId=302285</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -5958,12 +5955,12 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236976</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.amazon.in/dp/B0DZN2PGH2</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -6065,7 +6062,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>https://www.nykaa.com/l/p/626234</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -6102,12 +6099,12 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>568</t>
+          <t>https://www.nykaa.com/mak/p/6735650</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>https://www.amazon.in/dp/B08L9SVPBZ</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -6137,7 +6134,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>1439</t>
+          <t>https://www.nykaa.com/l/p/4308959?redirectpath=slug&amp;skuId=</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -6172,7 +6169,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/mak/p/3887831</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -6207,7 +6204,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>https://www.nykaa.com/makeup-revolution-fast-base-stick-foundation/p/302292?redirectpath=slug&amp;skuId=302280</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -6275,7 +6272,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>https://www.nykaa.com/revolution-relove-super-bronzer/p/4349381?productId=4349381&amp;pps=1&amp;skuId=4349363</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -6310,7 +6307,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=18236981</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -6345,12 +6342,12 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>https://www.nykaa.com/mak/p/2784817</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>https://www.amazon.in/dp/B095J5R77Q</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -6382,7 +6379,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>https://www.nykaa.com/l/p/18456056?redirectpath=slug&amp;skuId=18456047</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -6417,7 +6414,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>https://www.nykaa.com/mak/p/14235433</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -6454,7 +6451,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>880</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-setting-powder/p/81923?redirectpath=slug&amp;skuId=81879</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -6489,7 +6486,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=19993932</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -6526,12 +6523,12 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40874</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>651</t>
+          <t>https://www.amazon.in/dp/B007MJKI54</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -6563,7 +6560,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40868</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -6598,7 +6595,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=18236979</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -6633,12 +6630,12 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>638</t>
+          <t>https://www.nykaa.com/mak/p/15662740</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>656</t>
+          <t>https://www.amazon.in/dp/B0CT47M46T</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -6670,7 +6667,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/l-a-girl-luminous-glow-illuminating-cream/p/306042?productId=306042&amp;pps=1&amp;skuId=306041</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -6705,12 +6702,12 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=19232727</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>https://www.amazon.in/dp/B0DSWLY9L3</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -6740,12 +6737,12 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=19232728</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.amazon.in/dp/B0DZP1R2BV</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -6782,7 +6779,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>https://www.amazon.in/dp/B08P1SZFJ3</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -6849,7 +6846,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=12364250</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -6884,12 +6881,12 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>339</t>
+          <t>https://www.nykaa.com/makeup-revolution-relove-baby-gloss/p/8465698?redirectpath=slug&amp;skuId=8465692</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>https://www.amazon.in/dp/B095J4RT99</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -6921,7 +6918,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/focallure-fa-l27-star-studded-lip-gloss/p/17516496?productId=17516496&amp;pps=1&amp;skuId=17516472</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -6956,7 +6953,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>660</t>
+          <t>https://www.nykaa.com/mak/p/3887835</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -6993,12 +6990,12 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40865</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>https://www.amazon.in/dp/B009WHZXW2</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -7028,7 +7025,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>615</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=301723</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -7065,7 +7062,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>https://www.nykaa.com/mak/p/24807</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -7170,7 +7167,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>788</t>
+          <t>https://www.nykaa.com/makeup-revolution-ultra-blush-and-contour-palette/p/24735?redirectpath=slug&amp;skuId=24737</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -7205,7 +7202,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>https://www.nykaa.com/makeup-revolution-blusher-reloaded/p/540752?redirectpath=slug&amp;skuId=7667315</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -7242,7 +7239,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>https://www.nykaa.com/l/p/6735662?redirectpath=slug&amp;skuId=6735654</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -7277,12 +7274,12 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>https://www.nykaa.com/mak/p/2784807</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>https://www.amazon.in/dp/B095J3G3CZ</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -7314,7 +7311,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>https://www.nykaa.com/l/p/6735662?redirectpath=slug&amp;skuId=6735653</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -7349,7 +7346,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>https://www.nykaa.com/makeup-revolution-fast-base-stick-foundation/p/302292?redirectpath=slug&amp;skuId=302282</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -7384,7 +7381,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>https://www.nykaa.com/relove-super-matte-fix-mist/p/2784832?productId=2784832&amp;pps=1</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -7419,7 +7416,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>439</t>
+          <t>https://www.nykaa.com/relove-pore-vanish-prime-mist/p/2784819?productId=2784819&amp;pps=1</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -7489,12 +7486,12 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>https://www.nykaa.com/relove-colour-play-blushed-duo/p/3442503?redirectpath=slug&amp;skuId=2784790</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B095J49B18</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -7524,7 +7521,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>840</t>
+          <t>https://www.nykaa.com/mak/p/4512638</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -7559,12 +7556,12 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=18236980</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>https://www.amazon.in/dp/B0DHDCX159</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -7633,7 +7630,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>823</t>
+          <t>https://www.nykaa.com/focallure-airy-velvet-lipcream/p/17516493?productId=17516493&amp;pps=1&amp;skuId=17516457</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -7740,12 +7737,12 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/mak/p/8574500</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>1125</t>
+          <t>https://www.amazon.in/dp/B07HPDQ7PX</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -7812,7 +7809,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>1575</t>
+          <t>https://www.nykaa.com/mak/p/521058</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -7919,7 +7916,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/l/p/626233</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -7954,12 +7951,12 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/makeup-revolution-jelly-blush-stick/p/19145036?redirectpath=slug&amp;skuId=18283924</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DCZLTYCQ</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -8133,12 +8130,12 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>https://www.nykaa.com/makeup-revolution-mega-bronzer/p/3887841?redirectpath=slug&amp;skuId=465909</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B07QLMWGJD</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -8170,12 +8167,12 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>https://www.nykaa.com/mak/p/378198</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>1287</t>
+          <t>https://www.amazon.in/dp/B07HPFVH1K</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -8244,7 +8241,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81863</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -8353,7 +8350,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>https://www.nykaa.com/l/p/12179069?redirectpath=slug&amp;skuId=19993929</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -8390,12 +8387,12 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=378194</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>https://www.amazon.in/dp/B07HR4LN4P</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -8458,7 +8455,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>https://www.nykaa.com/relove-power-fix-primer/p/2784823?productId=2784823&amp;pps=1</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -8493,7 +8490,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>439</t>
+          <t>https://www.nykaa.com/relove-super-matte-primer/p/2784833?productId=2784833&amp;pps=1</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -8565,7 +8562,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236973</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -8637,12 +8634,12 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>https://www.nykaa.com/makeup-revolution-air-blur-matte-liquid-lipstick/p/19232732?redirectpath=slug&amp;skuId=18237974</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>https://www.amazon.in/dp/B0DSWM6VCR</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -8674,7 +8671,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>641</t>
+          <t>https://www.nykaa.com/l/p/6735662?redirectpath=slug&amp;skuId=6735657</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -8709,7 +8706,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236972</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -8744,12 +8741,12 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>1140</t>
+          <t>https://www.nykaa.com/revolution-pro-miracle-cream/p/18435841?productId=18435841&amp;pps=1</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>1140</t>
+          <t>https://www.amazon.in/dp/B09Z39NN2F</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -8812,7 +8809,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>615</t>
+          <t>https://www.nykaa.com/l/p/5072202?redirectpath=slug&amp;skuId=445862</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -8849,7 +8846,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>641</t>
+          <t>https://www.nykaa.com/l/p/6735662?redirectpath=slug&amp;skuId=6735658</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -8884,7 +8881,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>https://www.nykaa.com/makeup-revolution-juicy-peptide-lip-balm/p/17524139?redirectpath=slug&amp;skuId=17524136</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -8993,7 +8990,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>878</t>
+          <t>https://www.nykaa.com/mak/p/339713</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -9028,7 +9025,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>1063</t>
+          <t>https://www.nykaa.com/makeup-revolution-sss-foundation/p/18236978?redirectpath=slug&amp;skuId=18236975</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -9063,7 +9060,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>https://www.nykaa.com/mak/p/60999</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -9098,7 +9095,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>652</t>
+          <t>https://www.nykaa.com/makeup-revolution-fast-base-contour-stick/p/6832681?redirectpath=slug&amp;skuId=6832628</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -9135,7 +9132,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>https://www.nykaa.com/l/p/40862?redirectpath=slug&amp;skuId=40875</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -9209,7 +9206,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>https://www.nykaa.com/l-a-girl-hd-pro-bb-cream/p/41499?productId=41499&amp;pps=1&amp;skuId=41503</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -9353,12 +9350,12 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/focallure-fa-l27-star-studded-lip-gloss/p/17516496?productId=17516496&amp;pps=1&amp;skuId=17516471</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B08P1SFKML</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -9388,7 +9385,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>708</t>
+          <t>https://www.nykaa.com/makeup-revolution-beam-bright-highlighter/p/15662754?redirectpath=slug&amp;skuId=15662729</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -9423,7 +9420,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>https://www.nykaa.com/makeup-revolution-shimmer-bomb/p/8518930?productId=8518930&amp;pps=1&amp;skuId=8518902</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -9460,7 +9457,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>1233</t>
+          <t>https://www.nykaa.com/l-a-girl-pro-coverage-illuminating-liquid-foundation/p/81919?redirectpath=slug&amp;skuId=81866</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -9495,7 +9492,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>1318</t>
+          <t>https://www.nykaa.com/makeup-revolution-forever-flawless-palette/p/18283926?productId=18283926&amp;pps=1&amp;skuId=18283920</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -9530,7 +9527,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>https://www.nykaa.com/makeup-revolution-juicy-peptide-lip-balm/p/17524139?redirectpath=slug&amp;skuId=17524134</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -9604,7 +9601,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>https://www.nykaa.com/l/p/18456056?redirectpath=slug&amp;skuId=18456046</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -9674,7 +9671,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>https://www.nykaa.com/l/p/18456056?redirectpath=slug&amp;skuId=18456049</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -9711,7 +9708,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>https://www.nykaa.com/l/p/18456056?redirectpath=slug&amp;skuId=18456042</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -9748,7 +9745,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>880</t>
+          <t>https://www.nykaa.com/l/p/41508</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -9785,7 +9782,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>1610</t>
+          <t>https://www.nykaa.com/focallure-star-crash-stretchy-highlighter/p/19383040?productId=19383040&amp;pps=1&amp;skuId=19383023</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -9855,7 +9852,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>https://www.nykaa.com/l/p/18456056?redirectpath=slug&amp;skuId=18456043</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -9923,7 +9920,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>https://www.nykaa.com/mak/p/1130106</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -9958,12 +9955,12 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>https://www.nykaa.com/makeup-revolution-irl-filter-finish-concealer/p/11997546?productId=11997546&amp;pps=1&amp;skuId=11997541</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>https://www.amazon.in/dp/B0BQWWMTY2</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -10063,7 +10060,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>858</t>
+          <t>https://www.nykaa.com/makeup-revolution-superdewy-tinted-moisturiser/p/7667321?redirectpath=slug&amp;skuId=7667318</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -10100,7 +10097,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>1628</t>
+          <t>https://www.nykaa.com/l/p/8817444</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -10137,7 +10134,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>1665</t>
+          <t>https://www.nykaa.com/l-a-girl-18-color-eyeshadow-palette/p/20337205?redirectpath=slug&amp;skuId=5237374</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -10205,7 +10202,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>https://www.nykaa.com/mak/p/497426</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -10245,7 +10242,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0DWFR9FXQ</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10351,7 +10348,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>https://www.nykaa.com/focallure-fa-l27-star-studded-lip-gloss/p/17516496?productId=17516496&amp;pps=1&amp;skuId=17516473</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -10827,7 +10824,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.amazon.in/dp/B0CWRTPXB5</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">

</xml_diff>